<commit_message>
修改waffle chart 方案为multiple chart
</commit_message>
<xml_diff>
--- a/✈️可视化项目列表.xlsx
+++ b/✈️可视化项目列表.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="6360" yWindow="1760" windowWidth="33680" windowHeight="25560" tabRatio="500"/>
+    <workbookView xWindow="18440" yWindow="2100" windowWidth="41980" windowHeight="25560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="42">
   <si>
     <t>分镜头</t>
     <rPh sb="0" eb="1">
@@ -79,16 +79,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>机场中心度</t>
-    <rPh sb="0" eb="1">
-      <t>ji chang</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>zhong xin du</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>可视化形式</t>
     <rPh sb="0" eb="1">
       <t>ke shi hua</t>
@@ -104,45 +94,6 @@
   </si>
   <si>
     <t>mapboxgl</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>重点机场描述1</t>
-    <rPh sb="0" eb="1">
-      <t>zhong dian</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ji chang</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>miao shu</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>重点机场描述2</t>
-    <rPh sb="0" eb="1">
-      <t>zhong dian</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ji chang</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>miao shu</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>重点机场描述3</t>
-    <rPh sb="0" eb="1">
-      <t>zhong dian</t>
-    </rPh>
-    <rPh sb="2" eb="3">
-      <t>ji chang</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>miao shu</t>
-    </rPh>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -334,35 +285,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>机场中心度TOP10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Viewport Transition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Viewport Transition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Viewport Transition</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>空镜头，视觉过渡</t>
-    <rPh sb="0" eb="1">
-      <t>kong jing tou</t>
-    </rPh>
-    <rPh sb="4" eb="5">
-      <t>shi jue guo du</t>
-    </rPh>
-    <rPh sb="6" eb="7">
-      <t>guo du</t>
-    </rPh>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>交互式数据可视化（scatterplot+arcs）/boundle（静态大图）/空缺</t>
     <rPh sb="0" eb="1">
       <t>jiao hu</t>
@@ -382,19 +304,93 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>scatterplot(radius+color)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>linesLayer(opacity)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2018年机场中心度</t>
+    <rPh sb="4" eb="5">
+      <t>nian</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>ji chang</t>
+    </rPh>
+    <rPh sb="7" eb="8">
+      <t>zhong xin du</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>新疆省机场数量+航线+吞吐量</t>
+    <rPh sb="3" eb="4">
+      <t>ji chang</t>
+    </rPh>
+    <rPh sb="5" eb="6">
+      <t>shu liang</t>
+    </rPh>
+    <rPh sb="8" eb="9">
+      <t>hang x a</t>
+    </rPh>
+    <rPh sb="11" eb="12">
+      <t>tun tu liang</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>scatterplot(radius)+timeLine</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>scatterplot(radius+color)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>text/icon+arcs(animation)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>linesLayer(opacity)</t>
+    <t>Viewport Transition+arcs+scatterplot(radius)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015～2018机场中心度变化率TOP30</t>
+    <rPh sb="14" eb="15">
+      <t>bian hua lü</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2015～2018机场中心度变化率</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>historgram(animation)+mapboxLayer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机场名+变化率</t>
+    <rPh sb="0" eb="1">
+      <t>ji chang ming</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>bian hua lb</t>
+    </rPh>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>机场坐标+航线（OD*2*3）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>text/icon</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>老资历机场TOP10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Viewport Transition+arcs(animation)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>宁波栎社机场</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -854,16 +850,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I13"/>
+  <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="292" zoomScaleNormal="292" zoomScalePageLayoutView="292" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScale="162" zoomScaleNormal="162" zoomScalePageLayoutView="162" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="25.33203125" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="33.5" customWidth="1"/>
     <col min="4" max="4" width="33.6640625" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
   </cols>
@@ -876,25 +872,25 @@
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>9</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -905,10 +901,10 @@
         <v>4</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E2" t="s">
         <v>5</v>
@@ -923,7 +919,7 @@
         <v>5</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -934,10 +930,10 @@
         <v>7</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="D3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E3" t="s">
         <v>5</v>
@@ -952,100 +948,89 @@
         <v>6</v>
       </c>
       <c r="I3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" t="s">
+        <v>14</v>
+      </c>
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D4" t="s">
-        <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>6</v>
-      </c>
-      <c r="G4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
-        <v>3.5</v>
-      </c>
-      <c r="B5" s="3" t="s">
+      <c r="E6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G6" t="s">
+        <v>5</v>
+      </c>
+      <c r="H6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="5"/>
+    </row>
+    <row r="7" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>30</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" t="s">
-        <v>5</v>
-      </c>
-      <c r="F5" t="s">
-        <v>6</v>
-      </c>
-      <c r="G5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
-      <c r="I5" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>5</v>
-      </c>
-      <c r="G6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>13</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>32</v>
       </c>
       <c r="D7" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E7" t="s">
         <v>5</v>
@@ -1062,16 +1047,16 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E8" t="s">
         <v>5</v>
@@ -1087,55 +1072,55 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
-      <c r="F9" s="10"/>
-      <c r="G9" s="10"/>
-      <c r="H9" s="11"/>
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" t="s">
+        <v>5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>5</v>
+      </c>
+      <c r="H9" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="1">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
-      </c>
-      <c r="E10" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" t="s">
-        <v>6</v>
-      </c>
-      <c r="H10" t="s">
-        <v>5</v>
-      </c>
+      <c r="A10" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="11"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D11" t="s">
-        <v>28</v>
       </c>
       <c r="E11" t="s">
         <v>6</v>
@@ -1152,16 +1137,16 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
         <v>6</v>
@@ -1178,16 +1163,16 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
         <v>6</v>
@@ -1199,12 +1184,38 @@
         <v>6</v>
       </c>
       <c r="H13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A9:H9"/>
+    <mergeCell ref="A10:H10"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>